<commit_message>
Final plan and initial files.
</commit_message>
<xml_diff>
--- a/SquashPlanner.xlsx
+++ b/SquashPlanner.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
     <sheet name="Functions" sheetId="2" r:id="rId2"/>
     <sheet name="Files" sheetId="3" r:id="rId3"/>
+    <sheet name="DB_Functions" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="116">
   <si>
     <t>Honnan (HTML)</t>
   </si>
@@ -143,12 +144,6 @@
   </si>
   <si>
     <t>matches</t>
-  </si>
-  <si>
-    <t>player1_id</t>
-  </si>
-  <si>
-    <t>player2_id</t>
   </si>
   <si>
     <t>place_id</t>
@@ -281,14 +276,116 @@
     <t>Szilárd</t>
   </si>
   <si>
-    <t>Fájl</t>
+    <t>player1_email</t>
+  </si>
+  <si>
+    <t>player2_email</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>db</t>
+  </si>
+  <si>
+    <t>security_config</t>
+  </si>
+  <si>
+    <t>Function name</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>Returns</t>
+  </si>
+  <si>
+    <t>getAllUsers</t>
+  </si>
+  <si>
+    <t>List&lt;User&gt;</t>
+  </si>
+  <si>
+    <t>getUserByName</t>
+  </si>
+  <si>
+    <t>String name</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>addUser</t>
+  </si>
+  <si>
+    <t>User user</t>
+  </si>
+  <si>
+    <t>updateUser</t>
+  </si>
+  <si>
+    <t>removeUser</t>
+  </si>
+  <si>
+    <t>getAllPlaces</t>
+  </si>
+  <si>
+    <t>List&lt;Place&gt;</t>
+  </si>
+  <si>
+    <t>addPlace</t>
+  </si>
+  <si>
+    <t>Place place</t>
+  </si>
+  <si>
+    <t>updatePlace</t>
+  </si>
+  <si>
+    <t>removePlace</t>
+  </si>
+  <si>
+    <t>getAllMatches</t>
+  </si>
+  <si>
+    <t>List&lt;Match&gt;</t>
+  </si>
+  <si>
+    <t>getAllMatchesByUserId</t>
+  </si>
+  <si>
+    <t>int userId</t>
+  </si>
+  <si>
+    <t>getAllMatchesByPlaceId</t>
+  </si>
+  <si>
+    <t>int placeId</t>
+  </si>
+  <si>
+    <t>addMatch</t>
+  </si>
+  <si>
+    <t>Match match</t>
+  </si>
+  <si>
+    <t>updateMatch</t>
+  </si>
+  <si>
+    <t>removeMatch</t>
+  </si>
+  <si>
+    <t>encrypt</t>
+  </si>
+  <si>
+    <t>Fájl / Package</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,6 +409,23 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -341,7 +455,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -486,14 +600,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -514,14 +640,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -548,11 +670,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="40% - 4. jelölőszín" xfId="1" builtinId="43"/>
     <cellStyle name="40% - 5. jelölőszín" xfId="2" builtinId="47"/>
     <cellStyle name="40% - 6. jelölőszín" xfId="3" builtinId="51"/>
+    <cellStyle name="Magyarázó szöveg" xfId="4" builtinId="53"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -848,7 +979,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -858,30 +989,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1">
-      <c r="A1" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="28" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="16" t="s">
+      <c r="D2" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -890,10 +1017,7 @@
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -911,10 +1035,7 @@
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -932,10 +1053,7 @@
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="7"/>
@@ -951,28 +1069,27 @@
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1">
-      <c r="A6" s="11" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="13"/>
       <c r="G6" s="7"/>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1"/>
     <row r="9" spans="1:7" ht="15" thickBot="1">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="D9" s="28" t="s">
+      <c r="B9" s="23"/>
+      <c r="D9" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="30"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="6" t="s">
@@ -981,7 +1098,7 @@
       <c r="B10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="16" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -1048,37 +1165,37 @@
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1"/>
     <row r="15" spans="1:7" ht="15" thickBot="1">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="31"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="E16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="17" t="s">
         <v>43</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1101,7 +1218,7 @@
         <v>24</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1128,13 +1245,13 @@
         <v>29</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -1143,10 +1260,10 @@
     <row r="20" spans="1:7" ht="15" thickBot="1">
       <c r="A20" s="11"/>
       <c r="B20" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
@@ -1158,7 +1275,7 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="D9:G9"/>
     <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -1169,8 +1286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1207,8 +1324,8 @@
       <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="25" t="s">
-        <v>80</v>
+      <c r="H1" s="21" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" thickTop="1">
@@ -1234,7 +1351,7 @@
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="39" customHeight="1">
@@ -1260,7 +1377,7 @@
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="58.8" customHeight="1">
@@ -1268,10 +1385,10 @@
         <v>16</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="60.6" customHeight="1">
@@ -1279,10 +1396,10 @@
         <v>17</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="54" customHeight="1">
@@ -1290,10 +1407,10 @@
         <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="63.6" customHeight="1">
@@ -1301,25 +1418,25 @@
         <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="48" customHeight="1">
@@ -1327,25 +1444,25 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="32.4" customHeight="1">
@@ -1353,13 +1470,13 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -1371,7 +1488,7 @@
         <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="56.4" customHeight="1">
@@ -1379,37 +1496,37 @@
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F10" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1"/>
     <row r="12" spans="1:8" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" spans="1:8" ht="15" thickTop="1"/>
     <row r="14" spans="1:8" ht="45.6" customHeight="1">
@@ -1417,25 +1534,25 @@
         <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="63.6" customHeight="1">
@@ -1443,25 +1560,25 @@
         <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F15" t="s">
         <v>16</v>
       </c>
       <c r="G15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="100.8" customHeight="1">
@@ -1469,25 +1586,25 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1498,56 +1615,274 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="2" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.600000000000001" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" customHeight="1" thickTop="1">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" customHeight="1">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.6" customHeight="1">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="29.4" customHeight="1">
+      <c r="A6" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="25.8" customHeight="1" thickTop="1">
+    <row r="7" spans="1:2" ht="29.4" customHeight="1">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="29.4" customHeight="1">
+      <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="29.4" customHeight="1">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="3" width="45.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.600000000000001" thickBot="1">
+      <c r="A1" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickTop="1">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="25.8" customHeight="1">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="25.8" customHeight="1">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="25.8" customHeight="1">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Model layer is done.
</commit_message>
<xml_diff>
--- a/SquashPlanner.xlsx
+++ b/SquashPlanner.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEF5D28-53BB-FD4F-9CA4-D8AB2DCEFD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F2051B-68EF-5347-BBF5-D8DE8E820E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -460,6 +460,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -625,7 +631,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -677,6 +683,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent4" xfId="1" builtinId="43"/>
@@ -987,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1624,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1667,10 +1674,10 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="29" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
index endpoint added, plan table updated
</commit_message>
<xml_diff>
--- a/SquashPlanner.xlsx
+++ b/SquashPlanner.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CEA27F-4FD4-1048-9211-1B6155D18FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE7AF59-5EA6-BA4A-A038-2DDAC811B4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,6 +466,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -631,7 +637,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -684,6 +690,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent4" xfId="1" builtinId="43"/>
@@ -1300,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1406,13 +1419,18 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="60.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F5" t="s">
+      <c r="A5" s="30"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="30" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1428,28 +1446,28 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="63.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="30" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1631,8 +1649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1658,10 +1676,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="29" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1715,7 +1733,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Index html is almost fully functional plus minor bugfixes
</commit_message>
<xml_diff>
--- a/SquashPlanner.xlsx
+++ b/SquashPlanner.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE7AF59-5EA6-BA4A-A038-2DDAC811B4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A2883D-342F-C44E-B3DA-FCDFFE9F1D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="116">
   <si>
     <t>Honnan (HTML)</t>
   </si>
@@ -377,6 +377,9 @@
   </si>
   <si>
     <t>CONSTRAINT players_not_the_same CHECK player1_email &lt;&gt; player2_email</t>
+  </si>
+  <si>
+    <t>Dávid (SpringSecurity)</t>
   </si>
 </sst>
 </file>
@@ -435,7 +438,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,12 +469,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -637,7 +634,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -670,6 +667,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -688,13 +687,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1021,13 +1017,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" s="16" t="s">
@@ -1105,16 +1101,16 @@
     </row>
     <row r="8" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="D9" s="24" t="s">
+      <c r="B9" s="25"/>
+      <c r="D9" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="28"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
@@ -1166,10 +1162,10 @@
       <c r="D12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="22" t="s">
         <v>27</v>
       </c>
       <c r="G12" s="7" t="s">
@@ -1190,15 +1186,15 @@
     </row>
     <row r="14" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="29"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
@@ -1313,8 +1309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1356,55 +1352,55 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="23" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H3" t="s">
-        <v>78</v>
+      <c r="H3" s="23" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="58.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1419,18 +1415,18 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="60.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="23" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1446,28 +1442,28 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="63.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="32" t="s">
+      <c r="G7" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="23" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1498,28 +1494,28 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="32.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="23" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1668,18 +1664,18 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="23" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="23" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1692,10 +1688,10 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="23" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1716,10 +1712,10 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="23" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1732,7 +1728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>

</xml_diff>